<commit_message>
Add test for binance sample data
</commit_message>
<xml_diff>
--- a/testdata/binance/binance-yabc-sample.xlsx
+++ b/testdata/binance/binance-yabc-sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t xml:space="preserve">Date(UTC)</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t xml:space="preserve">SELL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.01</t>
   </si>
   <si>
     <t xml:space="preserve">ETH</t>
@@ -175,18 +178,18 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8367346938776"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.8010204081633"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.26530612244898"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="6.88265306122449"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.69387755102041"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.8061224489796"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.86224489795918"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.75"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.63775510204082"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.3418367346939"/>
   </cols>
@@ -236,22 +239,22 @@
       <c r="F2" s="0" t="n">
         <v>125</v>
       </c>
-      <c r="G2" s="0" t="n">
-        <v>0.01</v>
+      <c r="G2" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>0.008</v>
@@ -262,22 +265,22 @@
       <c r="F3" s="0" t="n">
         <v>125</v>
       </c>
-      <c r="G3" s="0" t="n">
-        <v>0.01</v>
+      <c r="G3" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>14</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>13</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>0.0001</v>
@@ -288,19 +291,19 @@
       <c r="F4" s="0" t="n">
         <v>10025</v>
       </c>
-      <c r="G4" s="0" t="n">
-        <v>0.01</v>
+      <c r="G4" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>10</v>
@@ -314,11 +317,11 @@
       <c r="F5" s="0" t="n">
         <v>10030</v>
       </c>
-      <c r="G5" s="0" t="n">
-        <v>0.01</v>
+      <c r="G5" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>